<commit_message>
Final Bars download for US stocks program
</commit_message>
<xml_diff>
--- a/Python_TWS_API_Historical_Data_Download/Python_TWS_API_Historical_Data_Download/Dowload_Duration_Calculation.xlsx
+++ b/Python_TWS_API_Historical_Data_Download/Python_TWS_API_Historical_Data_Download/Dowload_Duration_Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python TWS API\Python_TWS_API_Historical_Data_Download\Python_TWS_API_Historical_Data_Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1229204-D402-4794-ACFD-35D258CD13DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F6504A8-8C41-4A55-8C9F-E9D66F18FF59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{C2C0AFCD-EAED-4457-93E0-C5200AF3A8C0}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Total 30 min periods to complete</t>
   </si>
@@ -46,14 +47,46 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>One 30-minute download will take (secs)</t>
+  </si>
+  <si>
+    <t>Secs</t>
+  </si>
+  <si>
+    <t>Criteria:</t>
+  </si>
+  <si>
+    <t>20 day average volume: &gt;400,000</t>
+  </si>
+  <si>
+    <t>IPO: &gt; 1 year ago</t>
+  </si>
+  <si>
+    <t>Exchanges: all US - OTC</t>
+  </si>
+  <si>
+    <t>Price range: 1 - 499</t>
+  </si>
+  <si>
+    <t>Securty Type: != MLP Ltd Part</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,19 +431,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DC28F2-574F-4B86-8758-D2B505988BB4}">
-  <dimension ref="A2:P5"/>
+  <dimension ref="A2:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
@@ -421,24 +459,27 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>11</v>
+      </c>
       <c r="F3">
         <f>249*13</f>
         <v>3237</v>
       </c>
       <c r="J3">
-        <v>4000</v>
+        <v>1161</v>
       </c>
       <c r="M3">
         <f>F3*J3</f>
-        <v>12948000</v>
+        <v>3758157</v>
       </c>
       <c r="O3">
         <f>M3*180</f>
-        <v>2330640000</v>
+        <v>676468260</v>
       </c>
       <c r="P3">
         <f>O3/1024/1024</f>
-        <v>2222.6715087890625</v>
+        <v>645.13040542602539</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -457,6 +498,9 @@
       <c r="G4" t="s">
         <v>4</v>
       </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -477,16 +521,61 @@
         <f>((F3/$E$5)/144)</f>
         <v>0.22479166666666664</v>
       </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
       <c r="M5">
         <f>((M3/$E$5)/144)*24</f>
-        <v>21580</v>
+        <v>6263.5949999999993</v>
       </c>
       <c r="N5">
         <f>((M3/$E$5)/144)</f>
-        <v>899.16666666666663</v>
+        <v>260.98312499999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>M3*D3</f>
+        <v>41339727</v>
+      </c>
+      <c r="N7">
+        <f>M7/3600</f>
+        <v>11483.2575</v>
+      </c>
+      <c r="O7" s="1">
+        <f>N7/24</f>
+        <v>478.46906250000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>